<commit_message>
solved for the passworod problem. tweak issue with deleting strings. started on historical comp
</commit_message>
<xml_diff>
--- a/index_variable_name.xlsx
+++ b/index_variable_name.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\Credit Rating Model Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E7EF1D-2E3A-45D4-8A65-391888895F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B7ED73-085E-4CE7-9936-94CCE21AF5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E172CFD8-28E0-428F-963F-4ABCF211A1E6}"/>
   </bookViews>
@@ -117,9 +117,6 @@
     <t>Nominal GDP per capita (US$)</t>
   </si>
   <si>
-    <t>Nomina GDP (US$ bil)</t>
-  </si>
-  <si>
     <t>Average Growth t-5 to t+4 (%)</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Baseline Rating (~middle of IG &amp; HY)</t>
+  </si>
+  <si>
+    <t>Nominal GDP (US$ bil)</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249BA2A3-1F79-4943-940D-57C785565171}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -631,10 +631,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -642,10 +642,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -653,10 +653,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -664,10 +664,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -683,7 +683,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -691,10 +691,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -702,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -718,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -726,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -734,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -742,7 +742,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -750,10 +750,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -761,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -769,7 +769,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -777,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -785,10 +785,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -796,10 +796,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -807,10 +807,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,7 +818,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -826,7 +826,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -834,10 +834,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost completed peer comparison page
</commit_message>
<xml_diff>
--- a/index_variable_name.xlsx
+++ b/index_variable_name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B7ED73-085E-4CE7-9936-94CCE21AF5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0B7A8F-E5F4-4BD5-9613-0385DA4413EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E172CFD8-28E0-428F-963F-4ABCF211A1E6}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>Reserve Currency Status (1 = Yes, 0 = No)</t>
   </si>
   <si>
-    <t>Wealth (6%)</t>
-  </si>
-  <si>
     <t>Size (18%)</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Nominal GDP (US$ bil)</t>
+  </si>
+  <si>
+    <t>Wealth (5%)</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -631,10 +631,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -642,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -664,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -691,7 +691,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -750,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>42</v>
@@ -785,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
@@ -796,7 +796,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
@@ -807,7 +807,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
@@ -834,7 +834,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
         <v>51</v>

</xml_diff>